<commit_message>
kpi ok clinique pas fini
</commit_message>
<xml_diff>
--- a/suivi-fe/backend/templates/derogation-template.xlsx
+++ b/suivi-fe/backend/templates/derogation-template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://metallumindustries-my.sharepoint.com/personal/abdelhak_es-shih_kepmetal_com/Documents/Bureau/App/Clinique/suivi-fe/backend/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdel\Desktop\KEP\suivie-FE\suivi-fe\backend\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="11" documentId="8_{EACBF3DC-653A-4C6E-A721-C5F9CE160146}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CD31F6A0-AE0F-4086-AA94-8972B22D1C52}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{488A2A0F-AA95-4A9B-9BE2-CA43BB9A6F89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-16245" windowWidth="29040" windowHeight="15720" xr2:uid="{29E86407-766E-47F6-94AC-C3F0FEB367D4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{29E86407-766E-47F6-94AC-C3F0FEB367D4}"/>
   </bookViews>
   <sheets>
     <sheet name="page1" sheetId="1" r:id="rId1"/>
@@ -467,7 +467,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -494,9 +494,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -601,6 +598,12 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1071,428 +1074,428 @@
   <dimension ref="A1:D67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="4" width="24.6640625" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.44140625" style="1"/>
+    <col min="1" max="4" width="24.7109375" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="45"/>
-      <c r="B1" s="48" t="s">
+    <row r="1" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="44"/>
+      <c r="B1" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="48"/>
-      <c r="D1" s="22" t="s">
+      <c r="C1" s="47"/>
+      <c r="D1" s="21" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="46"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="23"/>
-    </row>
-    <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="47"/>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="24"/>
-    </row>
-    <row r="4" spans="1:4" s="3" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+    <row r="2" spans="1:4" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="45"/>
+      <c r="B2" s="48"/>
+      <c r="C2" s="48"/>
+      <c r="D2" s="22"/>
+    </row>
+    <row r="3" spans="1:4" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="46"/>
+      <c r="B3" s="49"/>
+      <c r="C3" s="49"/>
+      <c r="D3" s="23"/>
+    </row>
+    <row r="4" spans="1:4" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="14" t="s">
+      <c r="B4" s="51"/>
+      <c r="C4" s="13" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="6"/>
     </row>
-    <row r="5" spans="1:4" s="3" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
+    <row r="5" spans="1:4" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="9"/>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D5" s="10"/>
-    </row>
-    <row r="6" spans="1:4" s="3" customFormat="1" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="13" t="s">
+      <c r="D5" s="50"/>
+    </row>
+    <row r="6" spans="1:4" s="3" customFormat="1" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="12" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="7"/>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="8"/>
     </row>
-    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+    <row r="7" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="26"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="28"/>
-    </row>
-    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="29"/>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="31"/>
-    </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="31"/>
-    </row>
-    <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="29"/>
-      <c r="B10" s="30"/>
-      <c r="C10" s="30"/>
-      <c r="D10" s="31"/>
-    </row>
-    <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="29"/>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="31"/>
-    </row>
-    <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="29"/>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="31"/>
-    </row>
-    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="29"/>
-      <c r="B13" s="30"/>
-      <c r="C13" s="30"/>
-      <c r="D13" s="31"/>
-    </row>
-    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="29"/>
-      <c r="B14" s="30"/>
-      <c r="C14" s="30"/>
-      <c r="D14" s="31"/>
-    </row>
-    <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="29"/>
-      <c r="B15" s="30"/>
-      <c r="C15" s="30"/>
-      <c r="D15" s="31"/>
-    </row>
-    <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="29"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="30"/>
-      <c r="D16" s="31"/>
-    </row>
-    <row r="17" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="29"/>
-      <c r="B17" s="30"/>
-      <c r="C17" s="30"/>
-      <c r="D17" s="31"/>
-    </row>
-    <row r="18" spans="1:4" s="2" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="32"/>
-      <c r="B18" s="33"/>
-      <c r="C18" s="33"/>
-      <c r="D18" s="34"/>
-    </row>
-    <row r="19" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="25" t="s">
+      <c r="B7" s="25"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="27"/>
+    </row>
+    <row r="8" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="28"/>
+      <c r="B8" s="29"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="30"/>
+    </row>
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="28"/>
+      <c r="B9" s="29"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+    </row>
+    <row r="10" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="28"/>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+    </row>
+    <row r="11" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="28"/>
+      <c r="B11" s="29"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="30"/>
+    </row>
+    <row r="12" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="28"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
+    </row>
+    <row r="13" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="28"/>
+      <c r="B13" s="29"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="30"/>
+    </row>
+    <row r="14" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="28"/>
+      <c r="B14" s="29"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30"/>
+    </row>
+    <row r="15" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="28"/>
+      <c r="B15" s="29"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30"/>
+    </row>
+    <row r="16" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="28"/>
+      <c r="B16" s="29"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="30"/>
+    </row>
+    <row r="17" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="28"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
+    </row>
+    <row r="18" spans="1:4" s="2" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="31"/>
+      <c r="B18" s="32"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="33"/>
+    </row>
+    <row r="19" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="26"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="28"/>
-    </row>
-    <row r="20" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="29"/>
-      <c r="B20" s="30"/>
-      <c r="C20" s="30"/>
-      <c r="D20" s="31"/>
-    </row>
-    <row r="21" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="29"/>
-      <c r="B21" s="30"/>
-      <c r="C21" s="30"/>
-      <c r="D21" s="31"/>
-    </row>
-    <row r="22" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="29"/>
-      <c r="B22" s="30"/>
-      <c r="C22" s="30"/>
-      <c r="D22" s="31"/>
-    </row>
-    <row r="23" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="29"/>
-      <c r="B23" s="30"/>
-      <c r="C23" s="30"/>
-      <c r="D23" s="31"/>
-    </row>
-    <row r="24" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="29"/>
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="31"/>
-    </row>
-    <row r="25" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="29"/>
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="31"/>
-    </row>
-    <row r="26" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="29"/>
-      <c r="B26" s="30"/>
-      <c r="C26" s="30"/>
-      <c r="D26" s="31"/>
-    </row>
-    <row r="27" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="29"/>
-      <c r="B27" s="30"/>
-      <c r="C27" s="30"/>
-      <c r="D27" s="31"/>
-    </row>
-    <row r="28" spans="1:4" s="3" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="32"/>
-      <c r="B28" s="33"/>
-      <c r="C28" s="33"/>
-      <c r="D28" s="34"/>
-    </row>
-    <row r="29" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="25" t="s">
+      <c r="B19" s="25"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="27"/>
+    </row>
+    <row r="20" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="28"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="30"/>
+    </row>
+    <row r="21" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="28"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="30"/>
+    </row>
+    <row r="22" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="28"/>
+      <c r="B22" s="29"/>
+      <c r="C22" s="29"/>
+      <c r="D22" s="30"/>
+    </row>
+    <row r="23" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="28"/>
+      <c r="B23" s="29"/>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30"/>
+    </row>
+    <row r="24" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="28"/>
+      <c r="B24" s="29"/>
+      <c r="C24" s="29"/>
+      <c r="D24" s="30"/>
+    </row>
+    <row r="25" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="28"/>
+      <c r="B25" s="29"/>
+      <c r="C25" s="29"/>
+      <c r="D25" s="30"/>
+    </row>
+    <row r="26" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="28"/>
+      <c r="B26" s="29"/>
+      <c r="C26" s="29"/>
+      <c r="D26" s="30"/>
+    </row>
+    <row r="27" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="28"/>
+      <c r="B27" s="29"/>
+      <c r="C27" s="29"/>
+      <c r="D27" s="30"/>
+    </row>
+    <row r="28" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="31"/>
+      <c r="B28" s="32"/>
+      <c r="C28" s="32"/>
+      <c r="D28" s="33"/>
+    </row>
+    <row r="29" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="26"/>
-      <c r="C29" s="27"/>
-      <c r="D29" s="28"/>
-    </row>
-    <row r="30" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="31"/>
-    </row>
-    <row r="31" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="31"/>
-    </row>
-    <row r="32" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
-      <c r="B32" s="30"/>
-      <c r="C32" s="30"/>
-      <c r="D32" s="31"/>
-    </row>
-    <row r="33" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
-      <c r="B33" s="30"/>
-      <c r="C33" s="30"/>
-      <c r="D33" s="31"/>
-    </row>
-    <row r="34" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="29"/>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="31"/>
-    </row>
-    <row r="35" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="29"/>
-      <c r="B35" s="30"/>
-      <c r="C35" s="30"/>
-      <c r="D35" s="31"/>
-    </row>
-    <row r="36" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
-      <c r="B36" s="30"/>
-      <c r="C36" s="30"/>
-      <c r="D36" s="31"/>
-    </row>
-    <row r="37" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="29"/>
-      <c r="B37" s="30"/>
-      <c r="C37" s="30"/>
-      <c r="D37" s="31"/>
-    </row>
-    <row r="38" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="29"/>
-      <c r="B38" s="30"/>
-      <c r="C38" s="30"/>
-      <c r="D38" s="31"/>
-    </row>
-    <row r="39" spans="1:4" s="3" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="32"/>
-      <c r="B39" s="33"/>
-      <c r="C39" s="33"/>
-      <c r="D39" s="34"/>
-    </row>
-    <row r="40" spans="1:4" s="3" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="11" t="s">
+      <c r="B29" s="25"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="27"/>
+    </row>
+    <row r="30" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="28"/>
+      <c r="B30" s="29"/>
+      <c r="C30" s="29"/>
+      <c r="D30" s="30"/>
+    </row>
+    <row r="31" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="28"/>
+      <c r="B31" s="29"/>
+      <c r="C31" s="29"/>
+      <c r="D31" s="30"/>
+    </row>
+    <row r="32" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="28"/>
+      <c r="B32" s="29"/>
+      <c r="C32" s="29"/>
+      <c r="D32" s="30"/>
+    </row>
+    <row r="33" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="28"/>
+      <c r="B33" s="29"/>
+      <c r="C33" s="29"/>
+      <c r="D33" s="30"/>
+    </row>
+    <row r="34" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="28"/>
+      <c r="B34" s="29"/>
+      <c r="C34" s="29"/>
+      <c r="D34" s="30"/>
+    </row>
+    <row r="35" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="28"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="30"/>
+    </row>
+    <row r="36" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="28"/>
+      <c r="B36" s="29"/>
+      <c r="C36" s="29"/>
+      <c r="D36" s="30"/>
+    </row>
+    <row r="37" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="28"/>
+      <c r="B37" s="29"/>
+      <c r="C37" s="29"/>
+      <c r="D37" s="30"/>
+    </row>
+    <row r="38" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="28"/>
+      <c r="B38" s="29"/>
+      <c r="C38" s="29"/>
+      <c r="D38" s="30"/>
+    </row>
+    <row r="39" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="31"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="32"/>
+      <c r="D39" s="33"/>
+    </row>
+    <row r="40" spans="1:4" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B40" s="5"/>
-      <c r="C40" s="14" t="s">
+      <c r="C40" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="D40" s="21"/>
-    </row>
-    <row r="41" spans="1:4" s="3" customFormat="1" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="17" t="s">
+      <c r="D40" s="20"/>
+    </row>
+    <row r="41" spans="1:4" s="3" customFormat="1" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B41" s="18"/>
-      <c r="C41" s="19" t="s">
+      <c r="B41" s="17"/>
+      <c r="C41" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D41" s="20"/>
-    </row>
-    <row r="42" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="35" t="s">
+      <c r="D41" s="19"/>
+    </row>
+    <row r="42" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="B42" s="36"/>
-      <c r="C42" s="37"/>
-      <c r="D42" s="38"/>
-    </row>
-    <row r="43" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="39"/>
-      <c r="B43" s="40"/>
-      <c r="C43" s="40"/>
-      <c r="D43" s="41"/>
-    </row>
-    <row r="44" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="39"/>
-      <c r="B44" s="40"/>
-      <c r="C44" s="40"/>
-      <c r="D44" s="41"/>
-    </row>
-    <row r="45" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="39"/>
-      <c r="B45" s="40"/>
-      <c r="C45" s="40"/>
-      <c r="D45" s="41"/>
-    </row>
-    <row r="46" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="39"/>
-      <c r="B46" s="40"/>
-      <c r="C46" s="40"/>
-      <c r="D46" s="41"/>
-    </row>
-    <row r="47" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="39"/>
-      <c r="B47" s="40"/>
-      <c r="C47" s="40"/>
-      <c r="D47" s="41"/>
-    </row>
-    <row r="48" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="39"/>
-      <c r="B48" s="40"/>
-      <c r="C48" s="40"/>
-      <c r="D48" s="41"/>
-    </row>
-    <row r="49" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="39"/>
-      <c r="B49" s="40"/>
-      <c r="C49" s="40"/>
-      <c r="D49" s="41"/>
-    </row>
-    <row r="50" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="39"/>
-      <c r="B50" s="40"/>
-      <c r="C50" s="40"/>
-      <c r="D50" s="41"/>
-    </row>
-    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="39"/>
-      <c r="B51" s="40"/>
-      <c r="C51" s="40"/>
-      <c r="D51" s="41"/>
-    </row>
-    <row r="52" spans="1:4" s="3" customFormat="1" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="42"/>
-      <c r="B52" s="43"/>
-      <c r="C52" s="43"/>
-      <c r="D52" s="44"/>
-    </row>
-    <row r="53" spans="1:4" s="3" customFormat="1" ht="21.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="11" t="s">
+      <c r="B42" s="35"/>
+      <c r="C42" s="36"/>
+      <c r="D42" s="37"/>
+    </row>
+    <row r="43" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="38"/>
+      <c r="B43" s="39"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="40"/>
+    </row>
+    <row r="44" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="38"/>
+      <c r="B44" s="39"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="40"/>
+    </row>
+    <row r="45" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="38"/>
+      <c r="B45" s="39"/>
+      <c r="C45" s="39"/>
+      <c r="D45" s="40"/>
+    </row>
+    <row r="46" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="38"/>
+      <c r="B46" s="39"/>
+      <c r="C46" s="39"/>
+      <c r="D46" s="40"/>
+    </row>
+    <row r="47" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="38"/>
+      <c r="B47" s="39"/>
+      <c r="C47" s="39"/>
+      <c r="D47" s="40"/>
+    </row>
+    <row r="48" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="38"/>
+      <c r="B48" s="39"/>
+      <c r="C48" s="39"/>
+      <c r="D48" s="40"/>
+    </row>
+    <row r="49" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="38"/>
+      <c r="B49" s="39"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="40"/>
+    </row>
+    <row r="50" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="38"/>
+      <c r="B50" s="39"/>
+      <c r="C50" s="39"/>
+      <c r="D50" s="40"/>
+    </row>
+    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="38"/>
+      <c r="B51" s="39"/>
+      <c r="C51" s="39"/>
+      <c r="D51" s="40"/>
+    </row>
+    <row r="52" spans="1:4" s="3" customFormat="1" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="41"/>
+      <c r="B52" s="42"/>
+      <c r="C52" s="42"/>
+      <c r="D52" s="43"/>
+    </row>
+    <row r="53" spans="1:4" s="3" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="10" t="s">
         <v>4</v>
       </c>
       <c r="B53" s="5"/>
-      <c r="C53" s="14" t="s">
+      <c r="C53" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D53" s="6"/>
     </row>
-    <row r="54" spans="1:4" s="3" customFormat="1" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="17" t="s">
+    <row r="54" spans="1:4" s="3" customFormat="1" ht="21.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B54" s="18"/>
-      <c r="C54" s="19" t="s">
+      <c r="B54" s="17"/>
+      <c r="C54" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="D54" s="20"/>
-    </row>
-    <row r="55" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D54" s="19"/>
+    </row>
+    <row r="55" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
     </row>
-    <row r="56" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
     </row>
-    <row r="57" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
     </row>
-    <row r="58" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
     </row>
-    <row r="59" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
     </row>
-    <row r="60" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
     </row>
-    <row r="61" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
     </row>
-    <row r="62" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B62" s="4"/>
       <c r="C62" s="4"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B65" s="4"/>
       <c r="C65" s="4"/>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B66" s="4"/>
       <c r="C66" s="4"/>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B67" s="4"/>
       <c r="C67" s="4"/>
     </row>

</xml_diff>